<commit_message>
Fixed Problem with Entities
Needed to add Entity Framework to the CRUD program I have been working
on. Now working on fixing the problems with the controller classes as
well as adding more controller classes.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Status</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Finish setting up documentation files</t>
+  </si>
+  <si>
+    <t>Note When you deploy an application to a production web server, you must remove code that seeds the database.</t>
+  </si>
+  <si>
+    <t>Remove code that seeds the database in BlueScript</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -263,20 +269,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -287,7 +293,75 @@
     <cellStyle name="Note" xfId="1" builtinId="10"/>
     <cellStyle name="Style 1" xfId="2"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -310,16 +384,23 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -330,111 +411,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -540,14 +516,14 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleMedium12 2" pivot="0" count="8">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="totalRow" dxfId="17"/>
-      <tableStyleElement type="firstColumn" dxfId="16"/>
-      <tableStyleElement type="lastColumn" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -562,13 +538,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E25" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent6">
   <autoFilter ref="B4:E25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Task" dataDxfId="9"/>
-    <tableColumn id="2" name="Description" dataDxfId="10"/>
-    <tableColumn id="3" name="Due Date" dataDxfId="8"/>
-    <tableColumn id="5" name="Status" dataDxfId="11"/>
+    <tableColumn id="1" name="Task" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Due Date" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -867,7 +843,7 @@
   <dimension ref="A2:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -887,13 +863,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.9">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -905,16 +881,16 @@
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="3"/>
@@ -1016,11 +992,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="7"/>
+    <row r="12" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
@@ -1209,13 +1193,13 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Slight changes to Backlog
updating backlog to what I will get done this week.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Due Date</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -122,6 +119,15 @@
   </si>
   <si>
     <t>Includes: Characters, settings/locations, chapters</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>String counter</t>
+  </si>
+  <si>
+    <t>using regex, let user know how often a certain name comes up in their writing. (pre-miniproject 01)</t>
   </si>
 </sst>
 </file>
@@ -131,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +215,10 @@
       <name val="Segoe UI Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -278,7 +288,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -305,36 +315,43 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent6" xfId="5" builtinId="49"/>
@@ -345,6 +362,36 @@
     <cellStyle name="Style 1" xfId="2"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -357,7 +404,7 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -433,36 +480,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -590,13 +607,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent6">
-  <autoFilter ref="B4:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
+  <autoFilter ref="B4:E26"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Task" dataDxfId="3"/>
-    <tableColumn id="2" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" name="Due Date" dataDxfId="0"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="1" name="Task" dataDxfId="6"/>
+    <tableColumn id="2" name="Description" dataDxfId="5"/>
+    <tableColumn id="3" name="Week" dataDxfId="3"/>
+    <tableColumn id="5" name="Status" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -892,10 +909,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:M59"/>
+  <dimension ref="A2:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -903,7 +920,7 @@
     <col min="1" max="1" width="4.375" style="3" customWidth="1"/>
     <col min="2" max="2" width="25.625" style="11" customWidth="1"/>
     <col min="3" max="3" width="35.625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.75" style="19" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.25" style="3" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="3.875" style="3" customWidth="1"/>
@@ -915,34 +932,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.9">
-      <c r="B2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
-      <c r="D3" s="18"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="3"/>
@@ -950,357 +967,383 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="14">
-        <v>41465</v>
+      <c r="D5" s="22">
+        <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="25">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="54.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="14">
-        <v>41465</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="54.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="14">
-        <v>41466</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="14">
-        <v>41467</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="14">
-        <v>41474</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="14">
-        <v>41464</v>
+      <c r="D10" s="22" t="s">
+        <v>19</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10" t="s">
+    </row>
+    <row r="13" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="E13" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+      <c r="C14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="24" x14ac:dyDescent="0.35">
+      <c r="B15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E15" s="8" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="I15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="20"/>
+        <v>25</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="20"/>
+      <c r="D19" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="20"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D26" s="21"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D27" s="21"/>
+      <c r="D27" s="18"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D28" s="21"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D29" s="21"/>
+      <c r="D29" s="18"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D30" s="21"/>
+      <c r="D30" s="18"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D31" s="21"/>
+      <c r="D31" s="18"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D32" s="21"/>
+      <c r="D32" s="18"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="21"/>
+      <c r="D33" s="18"/>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D34" s="21"/>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D35" s="21"/>
+      <c r="D35" s="18"/>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D36" s="21"/>
+      <c r="D36" s="18"/>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D37" s="21"/>
+      <c r="D37" s="18"/>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D38" s="21"/>
+      <c r="D38" s="18"/>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D39" s="21"/>
+      <c r="D39" s="18"/>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D40" s="21"/>
+      <c r="D40" s="18"/>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D41" s="21"/>
+      <c r="D41" s="18"/>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D42" s="21"/>
+      <c r="D42" s="18"/>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D43" s="21"/>
+      <c r="D43" s="18"/>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D44" s="21"/>
+      <c r="D44" s="18"/>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D45" s="21"/>
+      <c r="D45" s="18"/>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D46" s="21"/>
+      <c r="D46" s="18"/>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D47" s="21"/>
+      <c r="D47" s="18"/>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D48" s="21"/>
+      <c r="D48" s="18"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" s="21"/>
+      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D50" s="21"/>
+      <c r="D50" s="18"/>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D51" s="21"/>
+      <c r="D51" s="18"/>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D52" s="21"/>
+      <c r="D52" s="18"/>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D53" s="21"/>
+      <c r="D53" s="18"/>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D54" s="21"/>
+      <c r="D54" s="18"/>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D55" s="21"/>
+      <c r="D55" s="18"/>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D56" s="21"/>
+      <c r="D56" s="18"/>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D57" s="21"/>
+      <c r="D57" s="18"/>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D58" s="21"/>
+      <c r="D58" s="18"/>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D59" s="21"/>
+      <c r="D59" s="18"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
-      <formula>"Completed"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
-      <formula>"Not Started"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E26">
       <formula1>"Not Started, Pending, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
CRUD and MiniProject01 updated
added details page to crud... getting problems with it at the time.
MiniProject01 still a work in progress.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="75" windowWidth="12045" windowHeight="12510"/>
+    <workbookView minimized="1" xWindow="12600" yWindow="75" windowWidth="12045" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="To-Do-List" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Status</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Refresh Yourself on CRUD</t>
   </si>
   <si>
-    <t>in ASP.NET MVC 3. This needs to be done ASAP</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>Some type of blue feather pen</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Finish setting up documentation files</t>
   </si>
   <si>
@@ -128,6 +122,15 @@
   </si>
   <si>
     <t>using regex, let user know how often a certain name comes up in their writing. (pre-miniproject 01)</t>
+  </si>
+  <si>
+    <t>Create Entities</t>
+  </si>
+  <si>
+    <t>According to assignment shown online</t>
+  </si>
+  <si>
+    <t>in ASP.NET MVC 3. This needs to be done ASAP  Where you left off: http://www.asp.net/mvc/tutorials/getting-started-with-ef-using-mvc/implementing-basic-crud-functionality-with-the-entity-framework-in-asp-net-mvc-application</t>
   </si>
 </sst>
 </file>
@@ -336,22 +339,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent6" xfId="5" builtinId="49"/>
@@ -364,33 +367,16 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -406,19 +392,6 @@
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -480,6 +453,36 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -607,13 +610,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
-  <autoFilter ref="B4:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent6">
+  <autoFilter ref="B4:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Task" dataDxfId="6"/>
-    <tableColumn id="2" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" name="Week" dataDxfId="3"/>
-    <tableColumn id="5" name="Status" dataDxfId="4"/>
+    <tableColumn id="1" name="Task" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Week" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -909,10 +912,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:M60"/>
+  <dimension ref="A2:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -932,13 +935,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.9">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -957,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>0</v>
@@ -967,14 +970,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="22">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="21">
         <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -984,249 +989,232 @@
       <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="54.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="65.25" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="21">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="21">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B7" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="25">
-        <v>1</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="54.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="22">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="D14" s="21"/>
+      <c r="E14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="10" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="24" x14ac:dyDescent="0.35">
-      <c r="B15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>2</v>
+      <c r="C15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="I15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>19</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D16" s="22"/>
       <c r="E16" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="23" t="s">
-        <v>19</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="22"/>
       <c r="E17" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="D18" s="22"/>
       <c r="E18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="D19" s="22"/>
       <c r="E19" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="D20" s="22"/>
       <c r="E20" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="8"/>
+      <c r="B22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="23"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="23"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D27" s="18"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D28" s="18"/>
@@ -1326,24 +1314,27 @@
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D60" s="18"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E27">
       <formula1>"Not Started, Pending, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
What I will be working on over the weekend
Updated backlog with what I will be working on over the weekend sense I
finished what I needed to get done during week one as well as what I
would like to work on during week two. One of the things I will be
working on is a document that shows everything that goes into front-end
development and why it has a lot of technical depth.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
   <si>
     <t>Status</t>
   </si>
@@ -133,7 +133,31 @@
     <t>The Welcome page, where you can login/sign up for Blue Script.</t>
   </si>
   <si>
-    <t>By layout I mean the HTML shown on all pages on Blue Script</t>
+    <t>Create Mockup for Characters page</t>
+  </si>
+  <si>
+    <t>Create Mockup for My Work page</t>
+  </si>
+  <si>
+    <t>Create Mockup for Home page</t>
+  </si>
+  <si>
+    <t>Create Mockup for Settings/Locations page</t>
+  </si>
+  <si>
+    <t>Create Mockup for Chapters page</t>
+  </si>
+  <si>
+    <t>By layout I mean the HTML shown on all pages on Blue Script based on mockups</t>
+  </si>
+  <si>
+    <t>Hi-fi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create outline of why Front-end has technical depth </t>
+  </si>
+  <si>
+    <t>This document will show everything that goes into the front-end of a website</t>
   </si>
 </sst>
 </file>
@@ -370,6 +394,36 @@
   <dxfs count="17">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -456,36 +510,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -613,13 +637,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent6">
-  <autoFilter ref="B4:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
+  <autoFilter ref="B4:E33"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Task" dataDxfId="3"/>
-    <tableColumn id="2" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" name="Week" dataDxfId="1"/>
-    <tableColumn id="5" name="Status" dataDxfId="0"/>
+    <tableColumn id="1" name="Task" dataDxfId="6"/>
+    <tableColumn id="2" name="Description" dataDxfId="5"/>
+    <tableColumn id="3" name="Week" dataDxfId="4"/>
+    <tableColumn id="5" name="Status" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -915,10 +939,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:M61"/>
+  <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1013,98 +1037,106 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="24">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="24">
+        <v>2</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="24">
+        <v>2</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="24">
+        <v>2</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="24">
+        <v>2</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B13" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="24">
+        <v>2</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C14" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="54.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="55.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="21">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="21">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="B15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="7" t="s">
@@ -1114,174 +1146,232 @@
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="21">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="21">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="8" t="s">
+      <c r="D22" s="22"/>
+      <c r="E22" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="13" t="s">
+    <row r="23" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
+      <c r="D23" s="22"/>
+      <c r="E23" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="22"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="E24" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="D25" s="22"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
+      <c r="B26" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="C26" s="13"/>
       <c r="D26" s="22"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="13"/>
+      <c r="B27" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="C27" s="13"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D28" s="18"/>
+      <c r="B28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D29" s="18"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="8"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D30" s="18"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D31" s="18"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="8"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D32" s="18"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="18"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D34" s="18"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D36" s="18"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D37" s="18"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D38" s="18"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D39" s="18"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D43" s="18"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D44" s="18"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D45" s="18"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D46" s="18"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D47" s="18"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D48" s="18"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">
@@ -1322,24 +1412,42 @@
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D61" s="18"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="18"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" s="18"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D64" s="18"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="18"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="18"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E33">
       <formula1>"Not Started, Pending, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Completed being a front-end document
also started working on home page mockup. Weekly summaries and backlog
have been updated.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -394,36 +394,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -510,6 +480,36 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -637,13 +637,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent6">
   <autoFilter ref="B4:E33"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Task" dataDxfId="6"/>
-    <tableColumn id="2" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" name="Week" dataDxfId="4"/>
-    <tableColumn id="5" name="Status" dataDxfId="3"/>
+    <tableColumn id="1" name="Task" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Week" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -941,8 +941,8 @@
   </sheetPr>
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1046,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1116,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1436,13 +1436,13 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Small changes to documentation
I got a lot of input on my mockups today and I am going to work on the
mockups more based on the input.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -942,7 +942,7 @@
   <dimension ref="A2:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Started on My Work page
backlog and weekly summaries updated
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -942,7 +942,7 @@
   <dimension ref="A2:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1060,7 +1060,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="8" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
After a lot of thinking...
I decided to make Blue-script a working blue print as the exciting
feature. Now I will begin researching on how to go about using HTML 5
and javascript to make a working mind map.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -941,8 +941,8 @@
   </sheetPr>
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1228,7 +1228,9 @@
       <c r="C22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="22">
+        <v>2</v>
+      </c>
       <c r="E22" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Found some mind mapping tools
also found some details on highlighting text with java script. I really
need to study up on things I can do with HTML.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>Status</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>This document will show everything that goes into the front-end of a website</t>
+  </si>
+  <si>
+    <t>Highlighting text using JavaScript</t>
   </si>
 </sst>
 </file>
@@ -941,8 +944,8 @@
   </sheetPr>
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
@@ -1302,10 +1305,16 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="13"/>
+      <c r="B29" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="C29" s="13"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="8"/>
+      <c r="D29" s="22">
+        <v>2</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="13"/>

</xml_diff>

<commit_message>
Continued researching and editing
looked into twitter bootstrap to help with the grid layout of the site.
Made changes to the pdf. updated backlog and weekly summaries.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>Status</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>Highlighting text using JavaScript</t>
+  </si>
+  <si>
+    <t>Clear current highlightswhen entering in new string to look for.</t>
   </si>
 </sst>
 </file>
@@ -944,8 +944,8 @@
   </sheetPr>
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -966,7 +966,7 @@
   <sheetData>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.9">
       <c r="B2" s="26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -984,13 +984,13 @@
     <row r="4" spans="1:13" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>0</v>
@@ -1000,327 +1000,335 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="21">
         <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="24">
         <v>1</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="24">
         <v>2</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="24">
         <v>2</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="24">
         <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="24">
         <v>2</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="24">
         <v>2</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="D13" s="24">
         <v>2</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="55.5" x14ac:dyDescent="0.35">
       <c r="B15" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I15" s="2"/>
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="21">
         <v>1</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="21">
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="22"/>
       <c r="E24" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="D25" s="22">
+        <v>3</v>
+      </c>
       <c r="E25" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="22"/>
       <c r="E26" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="22"/>
       <c r="E27" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="22">
         <v>2</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="13"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B30" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="8"/>
+      <c r="D30" s="22">
+        <v>3</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="13"/>

</xml_diff>

<commit_message>
updated this weeks tasks
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t>Status</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Pending</t>
+  </si>
+  <si>
     <t>Task</t>
   </si>
   <si>
@@ -160,7 +163,10 @@
     <t>Highlighting text using JavaScript</t>
   </si>
   <si>
-    <t>Clear current highlightswhen entering in new string to look for.</t>
+    <t>Clear current highlights when entering in new string to look for.</t>
+  </si>
+  <si>
+    <t>implement drag and drop</t>
   </si>
 </sst>
 </file>
@@ -944,8 +950,8 @@
   </sheetPr>
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -966,7 +972,7 @@
   <sheetData>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.9">
       <c r="B2" s="26" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -984,13 +990,13 @@
     <row r="4" spans="1:13" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>0</v>
@@ -1000,341 +1006,341 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="21">
         <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="24">
         <v>1</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="24">
         <v>2</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="24">
         <v>2</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="24">
         <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="24">
         <v>2</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="24">
         <v>2</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" s="24">
         <v>2</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="55.5" x14ac:dyDescent="0.35">
       <c r="B15" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I15" s="2"/>
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="21">
         <v>1</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="21">
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="22">
-        <v>3</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D22" s="22"/>
       <c r="E22" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="22"/>
       <c r="E24" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="22">
-        <v>3</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D25" s="22"/>
       <c r="E25" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="22"/>
       <c r="E26" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="22"/>
       <c r="E27" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="22">
         <v>2</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="22">
+      <c r="D30" s="22"/>
+      <c r="E30" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="22">
         <v>3</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="13"/>

</xml_diff>

<commit_message>
Working on create new scene function
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -373,16 +373,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent6" xfId="5" builtinId="49"/>
@@ -393,36 +393,6 @@
     <cellStyle name="Style 1" xfId="2"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -511,6 +481,36 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -638,13 +638,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E28" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E28" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent6">
   <autoFilter ref="B4:E28"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Task" dataDxfId="6"/>
-    <tableColumn id="2" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" name="Week" dataDxfId="4"/>
-    <tableColumn id="5" name="Status" dataDxfId="3"/>
+    <tableColumn id="1" name="Task" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Week" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -942,8 +942,8 @@
   </sheetPr>
   <dimension ref="A2:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -963,13 +963,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="52.5" x14ac:dyDescent="0.9">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
@@ -1263,52 +1263,52 @@
       </c>
     </row>
     <row r="25" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="26">
         <v>4</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="27" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="26">
         <v>4</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
+      <c r="B27" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="26">
+        <v>4</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
-      <c r="B27" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="27">
-        <v>4</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D29" s="18"/>
@@ -1405,13 +1405,13 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
setting up characters as checkboxes
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Status</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Make all terms used in the website relatable to writers</t>
+  </si>
+  <si>
+    <t>Stats View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calulate and view many different stats (look at proposal) </t>
   </si>
 </sst>
 </file>
@@ -943,7 +949,7 @@
   <dimension ref="A2:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1159,9 +1165,7 @@
       <c r="C16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="20">
-        <v>5</v>
-      </c>
+      <c r="D16" s="20"/>
       <c r="E16" s="7" t="s">
         <v>10</v>
       </c>
@@ -1306,11 +1310,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
+    <row r="28" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B28" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="26">
+        <v>5</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D29" s="18"/>

</xml_diff>

<commit_message>
adding characters and settings now works
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Status</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Highlighting text using JavaScript</t>
   </si>
   <si>
-    <t>Clear current highlights when entering in new string to look for.</t>
-  </si>
-  <si>
     <t>implement drag and drop</t>
   </si>
   <si>
@@ -161,6 +158,12 @@
   </si>
   <si>
     <t xml:space="preserve">Calulate and view many different stats (look at proposal) </t>
+  </si>
+  <si>
+    <t>4 : 9 = 44%   4 complete : 5 incomplete</t>
+  </si>
+  <si>
+    <t>auto save feature</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
     <cellStyle name="Note" xfId="1" builtinId="10"/>
     <cellStyle name="Style 1" xfId="2"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -519,36 +522,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="7" tint="0.59999389629810485"/>
@@ -652,14 +625,14 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleMedium12 2" pivot="0" count="8">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="totalRow" dxfId="17"/>
-      <tableStyleElement type="firstColumn" dxfId="16"/>
-      <tableStyleElement type="lastColumn" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -674,8 +647,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
-  <autoFilter ref="B4:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E31" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
+  <autoFilter ref="B4:E31"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Task" dataDxfId="6"/>
     <tableColumn id="2" name="Description" dataDxfId="5"/>
@@ -976,10 +949,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:M58"/>
+  <dimension ref="A2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1230,10 +1203,10 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>36</v>
       </c>
       <c r="D19" s="21">
         <v>6</v>
@@ -1254,34 +1227,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="21"/>
+      <c r="D21" s="21">
+        <v>3</v>
+      </c>
       <c r="E21" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="D22" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="D23" s="21">
         <v>4</v>
@@ -1290,71 +1267,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="13" t="s">
+    <row r="24" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="21">
+      <c r="C24" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="26">
         <v>4</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="E24" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B25" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" s="26">
         <v>4</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
       <c r="B26" s="25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D26" s="26">
         <v>4</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B27" s="25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>48</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C28" s="25"/>
       <c r="D28" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E28" s="27" t="s">
         <v>2</v>
@@ -1379,57 +1354,57 @@
       <c r="E31" s="27"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="D33" s="18"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D34" s="18"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D36" s="18"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D37" s="18"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D38" s="18"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D39" s="18"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D43" s="18"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D44" s="18"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D45" s="18"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D46" s="18"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D47" s="18"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D48" s="18"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">
@@ -1458,27 +1433,24 @@
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D57" s="18"/>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D58" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E31">
       <formula1>"Not Started, Pending, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
changing sizes of divs
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -404,36 +404,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -520,6 +490,36 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -647,13 +647,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E31" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E31" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowCellStyle="Accent6">
   <autoFilter ref="B4:E31"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Task" dataDxfId="6"/>
-    <tableColumn id="2" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" name="Week" dataDxfId="4"/>
-    <tableColumn id="5" name="Status" dataDxfId="3"/>
+    <tableColumn id="1" name="Task" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Week" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -951,8 +951,8 @@
   </sheetPr>
   <dimension ref="A2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1278,7 +1278,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
@@ -1306,7 +1306,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
@@ -1439,13 +1439,13 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
working on the design of the home page
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -82,9 +82,6 @@
     <t xml:space="preserve">in ASP.NET MVC 3. This needs to be done ASAP </t>
   </si>
   <si>
-    <t>The Welcome page, where you can login/sign up for Blue Script.</t>
-  </si>
-  <si>
     <t>Create Mockup for Characters page</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>auto save feature</t>
+  </si>
+  <si>
+    <t>The Welcome page</t>
   </si>
 </sst>
 </file>
@@ -951,8 +951,8 @@
   </sheetPr>
   <dimension ref="A2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1049,10 +1049,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="23">
         <v>2</v>
@@ -1063,10 +1063,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="23">
         <v>2</v>
@@ -1077,10 +1077,10 @@
     </row>
     <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="23">
         <v>2</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="23">
         <v>2</v>
@@ -1105,10 +1105,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="23">
         <v>2</v>
@@ -1119,10 +1119,10 @@
     </row>
     <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="D13" s="23">
         <v>2</v>
@@ -1173,12 +1173,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D17" s="21">
         <v>6</v>
@@ -1192,32 +1192,32 @@
         <v>15</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="21">
         <v>6</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="D19" s="21">
         <v>6</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="21">
@@ -1229,7 +1229,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="21">
@@ -1241,10 +1241,10 @@
     </row>
     <row r="22" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="21">
         <v>4</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="23" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="21">
         <v>4</v>
@@ -1269,10 +1269,10 @@
     </row>
     <row r="24" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B24" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="25" t="s">
         <v>38</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>39</v>
       </c>
       <c r="D24" s="26">
         <v>4</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="25" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B25" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>40</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>41</v>
       </c>
       <c r="D25" s="26">
         <v>4</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="26" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
       <c r="B26" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>43</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>44</v>
       </c>
       <c r="D26" s="26">
         <v>4</v>
@@ -1311,10 +1311,10 @@
     </row>
     <row r="27" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B27" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="25" t="s">
         <v>46</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>47</v>
       </c>
       <c r="D27" s="26">
         <v>5</v>
@@ -1325,14 +1325,14 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="26">
         <v>6</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
@@ -1358,7 +1358,7 @@
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="18"/>
     </row>

</xml_diff>

<commit_message>
finishing home page and
testing cross browser
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Status</t>
   </si>
@@ -157,13 +157,25 @@
     <t xml:space="preserve">Calulate and view many different stats (look at proposal) </t>
   </si>
   <si>
-    <t>4 : 9 = 44%   4 complete : 5 incomplete</t>
-  </si>
-  <si>
     <t>auto save feature</t>
   </si>
   <si>
     <t>The Welcome page</t>
+  </si>
+  <si>
+    <t>Chapters page</t>
+  </si>
+  <si>
+    <t>task list</t>
+  </si>
+  <si>
+    <t>added to my blue script page</t>
+  </si>
+  <si>
+    <t>create slideshow</t>
+  </si>
+  <si>
+    <t>for home page</t>
   </si>
 </sst>
 </file>
@@ -951,8 +963,8 @@
   </sheetPr>
   <dimension ref="A2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1168,7 +1180,9 @@
       <c r="C16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="20">
+        <v>7</v>
+      </c>
       <c r="E16" s="7" t="s">
         <v>10</v>
       </c>
@@ -1178,7 +1192,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="21">
         <v>6</v>
@@ -1325,7 +1339,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="26">
@@ -1336,75 +1350,94 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="25"/>
+      <c r="B29" s="25" t="s">
+        <v>49</v>
+      </c>
       <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
+      <c r="D29" s="26">
+        <v>7</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="27"/>
+      <c r="B30" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="26">
+        <v>7</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="27"/>
+      <c r="B31" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="26">
+        <v>7</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D32" s="18"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C33" s="11" t="s">
-        <v>47</v>
-      </c>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="18"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="18"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="18"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" s="18"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="18"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="18"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" s="18"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" s="18"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" s="18"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="18"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" s="18"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" s="18"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
small problems with cross browser
and character names not saving... this was working earlier..
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -963,8 +963,8 @@
   </sheetPr>
   <dimension ref="A2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1198,7 +1198,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Talked to Tim backlog updated
a lot of work ahead this week.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/ProjectBacklog.xlsx
+++ b/DOCUMENTATION/ProjectBacklog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>Status</t>
   </si>
@@ -46,27 +46,18 @@
     <t>Design Logo for BlueScript</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Some type of blue feather pen</t>
   </si>
   <si>
     <t>Finish setting up documentation files</t>
   </si>
   <si>
-    <t>Implement Security</t>
-  </si>
-  <si>
     <t>Create Home page</t>
   </si>
   <si>
     <t>Create basic layout of BlueScript</t>
   </si>
   <si>
-    <t>Start simple</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -163,13 +154,19 @@
     <t>The Welcome page</t>
   </si>
   <si>
-    <t>create slideshow</t>
-  </si>
-  <si>
-    <t>for home page</t>
-  </si>
-  <si>
     <t>fix ajax</t>
+  </si>
+  <si>
+    <t>projects page</t>
+  </si>
+  <si>
+    <t>the starting point for the website, add new project, edit your projects and delete projects.</t>
+  </si>
+  <si>
+    <t>chapters page</t>
+  </si>
+  <si>
+    <t>page for writers to write chapters without distraction.</t>
   </si>
 </sst>
 </file>
@@ -955,10 +952,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:M56"/>
+  <dimension ref="A2:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1003,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>0</v>
@@ -1013,10 +1010,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="20">
         <v>1</v>
@@ -1041,10 +1038,10 @@
     </row>
     <row r="7" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" s="23">
         <v>1</v>
@@ -1055,10 +1052,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="23">
         <v>2</v>
@@ -1069,10 +1066,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="23">
         <v>2</v>
@@ -1083,10 +1080,10 @@
     </row>
     <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="23">
         <v>2</v>
@@ -1097,10 +1094,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="23">
         <v>2</v>
@@ -1111,10 +1108,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12" s="23">
         <v>2</v>
@@ -1125,10 +1122,10 @@
     </row>
     <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="23">
         <v>2</v>
@@ -1142,7 +1139,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" s="20">
         <v>1</v>
@@ -1156,7 +1153,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="20">
         <v>1</v>
@@ -1168,25 +1165,25 @@
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="21">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="20">
-        <v>7</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="C17" s="13" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D17" s="21">
         <v>6</v>
@@ -1195,12 +1192,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D18" s="21">
         <v>6</v>
@@ -1211,13 +1208,11 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>34</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C19" s="13"/>
       <c r="D19" s="21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>8</v>
@@ -1225,34 +1220,36 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="13"/>
+      <c r="C21" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="D21" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D22" s="21">
         <v>4</v>
@@ -1261,26 +1258,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
-      <c r="B23" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="13" t="s">
+    <row r="23" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="26">
+        <v>4</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="B24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="21">
-        <v>4</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="25" t="s">
+      <c r="C24" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>38</v>
       </c>
       <c r="D24" s="26">
         <v>4</v>
@@ -1289,7 +1286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
       <c r="B25" s="25" t="s">
         <v>39</v>
       </c>
@@ -1303,7 +1300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="44.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B26" s="25" t="s">
         <v>42</v>
       </c>
@@ -1311,21 +1308,19 @@
         <v>43</v>
       </c>
       <c r="D26" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>46</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C27" s="25"/>
       <c r="D27" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E27" s="27" t="s">
         <v>8</v>
@@ -1333,21 +1328,23 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B29" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="25"/>
+        <v>47</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="D29" s="26">
         <v>7</v>
       </c>
@@ -1355,7 +1352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B30" s="25" t="s">
         <v>49</v>
       </c>
@@ -1443,9 +1440,6 @@
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D55" s="18"/>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D56" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>